<commit_message>
Interface: add function integration
</commit_message>
<xml_diff>
--- a/Teachers-Bday.xlsx
+++ b/Teachers-Bday.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8415" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -55,10 +55,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -388,15 +387,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G156"/>
+  <dimension ref="A1:G157"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="B161" sqref="A156:B161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col width="17.85546875" customWidth="1" min="1" max="1"/>
+    <col width="17.88671875" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
     <col width="10" customWidth="1" min="5" max="22"/>
   </cols>
@@ -415,2020 +414,2031 @@
       <c r="G1" s="1" t="n"/>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="3" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>בן יצחק אפרת</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>8/9</t>
         </is>
       </c>
-      <c r="G2" s="3" t="n"/>
+      <c r="G2" s="2" t="n"/>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>ביביטקו מירה</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>12/9</t>
         </is>
       </c>
-      <c r="G3" s="3" t="n"/>
+      <c r="G3" s="2" t="n"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="3" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>הירשפלד רויטל</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>16/9</t>
         </is>
       </c>
-      <c r="G4" s="3" t="n"/>
+      <c r="G4" s="2" t="n"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="3" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>קורן בנאקוט אביטל</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>20/9</t>
         </is>
       </c>
-      <c r="G5" s="3" t="n"/>
+      <c r="G5" s="2" t="n"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="3" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>ברקוביץ חגית</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>22/9</t>
         </is>
       </c>
-      <c r="G6" s="3" t="n"/>
+      <c r="G6" s="2" t="n"/>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>ארבל עדי</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>23/9</t>
         </is>
       </c>
-      <c r="G7" s="3" t="n"/>
+      <c r="G7" s="2" t="n"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>דולב שירלי</t>
         </is>
       </c>
-      <c r="B8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>25/9</t>
         </is>
       </c>
-      <c r="G8" s="3" t="n"/>
+      <c r="G8" s="2" t="n"/>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>קסלר מיכל</t>
         </is>
       </c>
-      <c r="B9" s="3" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>28/9</t>
         </is>
       </c>
-      <c r="G9" s="3" t="n"/>
+      <c r="G9" s="2" t="n"/>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="3" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>פלדמן משה</t>
         </is>
       </c>
-      <c r="B10" s="3" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>2/10</t>
         </is>
       </c>
-      <c r="G10" s="3" t="n"/>
+      <c r="G10" s="2" t="n"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="3" t="inlineStr">
+      <c r="A11" s="2" t="inlineStr">
         <is>
           <t>צוקרמן דורית</t>
         </is>
       </c>
-      <c r="B11" s="3" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>4/10</t>
         </is>
       </c>
-      <c r="G11" s="3" t="n"/>
+      <c r="G11" s="2" t="n"/>
     </row>
     <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="3" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>עזר שמחה</t>
         </is>
       </c>
-      <c r="B12" s="3" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>6/10</t>
         </is>
       </c>
-      <c r="G12" s="3" t="n"/>
+      <c r="G12" s="2" t="n"/>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="3" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
         <is>
           <t>בראל שלי</t>
         </is>
       </c>
-      <c r="B13" s="3" t="inlineStr">
+      <c r="B13" s="2" t="inlineStr">
         <is>
           <t>7/10</t>
         </is>
       </c>
-      <c r="G13" s="3" t="n"/>
+      <c r="G13" s="2" t="n"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="3" t="inlineStr">
+      <c r="A14" s="2" t="inlineStr">
         <is>
           <t>גבעתי אורלי</t>
         </is>
       </c>
-      <c r="B14" s="3" t="inlineStr">
+      <c r="B14" s="2" t="inlineStr">
         <is>
           <t>12/10</t>
         </is>
       </c>
-      <c r="G14" s="3" t="n"/>
+      <c r="G14" s="2" t="n"/>
     </row>
     <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="3" t="inlineStr">
+      <c r="A15" s="2" t="inlineStr">
         <is>
           <t>פרץ שרון</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>14/10</t>
         </is>
       </c>
-      <c r="G15" s="3" t="n"/>
+      <c r="G15" s="2" t="n"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="3" t="inlineStr">
+      <c r="A16" s="2" t="inlineStr">
         <is>
           <t>טולצ'ינסקי רותי</t>
         </is>
       </c>
-      <c r="B16" s="3" t="inlineStr">
+      <c r="B16" s="2" t="inlineStr">
         <is>
           <t>21/10</t>
         </is>
       </c>
-      <c r="G16" s="3" t="n"/>
+      <c r="G16" s="2" t="n"/>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="3" t="inlineStr">
+      <c r="A17" s="2" t="inlineStr">
         <is>
           <t>אלפסי אורלי</t>
         </is>
       </c>
-      <c r="B17" s="3" t="inlineStr">
+      <c r="B17" s="2" t="inlineStr">
         <is>
           <t>22/10</t>
         </is>
       </c>
-      <c r="G17" s="3" t="n"/>
+      <c r="G17" s="2" t="n"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="3" t="inlineStr">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>שטרן אילנה</t>
         </is>
       </c>
-      <c r="B18" s="3" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>23/10</t>
         </is>
       </c>
-      <c r="G18" s="3" t="n"/>
+      <c r="G18" s="2" t="n"/>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="A19" s="2" t="inlineStr">
         <is>
           <t>גרינפלד סיגל</t>
         </is>
       </c>
-      <c r="B19" s="3" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
         <is>
           <t>24/10</t>
         </is>
       </c>
-      <c r="G19" s="3" t="n"/>
+      <c r="G19" s="2" t="n"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="3" t="inlineStr">
+      <c r="A20" s="2" t="inlineStr">
         <is>
           <t>גינדי איריס</t>
         </is>
       </c>
-      <c r="B20" s="3" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
         <is>
           <t>25/10</t>
         </is>
       </c>
-      <c r="G20" s="3" t="n"/>
+      <c r="G20" s="2" t="n"/>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="3" t="inlineStr">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>שוצמן יעקב</t>
         </is>
       </c>
-      <c r="B21" s="3" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>27/10</t>
         </is>
       </c>
-      <c r="G21" s="3" t="n"/>
+      <c r="G21" s="2" t="n"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="3" t="inlineStr">
+      <c r="A22" s="2" t="inlineStr">
         <is>
           <t>בנבנישתי נינה</t>
         </is>
       </c>
-      <c r="B22" s="3" t="inlineStr">
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>28/10</t>
         </is>
       </c>
-      <c r="G22" s="3" t="n"/>
+      <c r="G22" s="2" t="n"/>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="3" t="inlineStr">
+      <c r="A23" s="2" t="inlineStr">
         <is>
           <t>גינוסר סנדרה</t>
         </is>
       </c>
-      <c r="B23" s="3" t="inlineStr">
+      <c r="B23" s="2" t="inlineStr">
         <is>
           <t>3/11</t>
         </is>
       </c>
-      <c r="G23" s="3" t="n"/>
+      <c r="G23" s="2" t="n"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="3" t="inlineStr">
+      <c r="A24" s="2" t="inlineStr">
         <is>
           <t>דנינו אלקיים לימור</t>
         </is>
       </c>
-      <c r="B24" s="3" t="inlineStr">
+      <c r="B24" s="2" t="inlineStr">
         <is>
           <t>3/11</t>
         </is>
       </c>
-      <c r="G24" s="3" t="n"/>
+      <c r="G24" s="2" t="n"/>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="3" t="inlineStr">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>בוהדנה נירה</t>
         </is>
       </c>
-      <c r="B25" s="3" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>5/11</t>
         </is>
       </c>
-      <c r="G25" s="3" t="n"/>
+      <c r="G25" s="2" t="n"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="3" t="inlineStr">
+      <c r="A26" s="2" t="inlineStr">
         <is>
           <t>ויליגר בן ציון</t>
         </is>
       </c>
-      <c r="B26" s="3" t="inlineStr">
+      <c r="B26" s="2" t="inlineStr">
         <is>
           <t>7/11</t>
         </is>
       </c>
-      <c r="G26" s="3" t="n"/>
+      <c r="G26" s="2" t="n"/>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="3" t="inlineStr">
+      <c r="A27" s="2" t="inlineStr">
         <is>
           <t>יחזקאל גולן</t>
         </is>
       </c>
-      <c r="B27" s="3" t="inlineStr">
+      <c r="B27" s="2" t="inlineStr">
         <is>
           <t>9/11</t>
         </is>
       </c>
-      <c r="G27" s="3" t="n"/>
+      <c r="G27" s="2" t="n"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="3" t="inlineStr">
+      <c r="A28" s="2" t="inlineStr">
         <is>
           <t>גולן יפעת</t>
         </is>
       </c>
-      <c r="B28" s="3" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>10/11</t>
         </is>
       </c>
-      <c r="G28" s="3" t="n"/>
+      <c r="G28" s="2" t="n"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="3" t="inlineStr">
+      <c r="A29" s="2" t="inlineStr">
         <is>
           <t>נגר יוסי</t>
         </is>
       </c>
-      <c r="B29" s="3" t="inlineStr">
+      <c r="B29" s="2" t="inlineStr">
         <is>
           <t>10/11</t>
         </is>
       </c>
-      <c r="G29" s="3" t="n"/>
+      <c r="G29" s="2" t="n"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="3" t="inlineStr">
+      <c r="A30" s="2" t="inlineStr">
         <is>
           <t>בר נתן טל</t>
         </is>
       </c>
-      <c r="B30" s="3" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
         <is>
           <t>13/11</t>
         </is>
       </c>
-      <c r="G30" s="3" t="n"/>
+      <c r="G30" s="2" t="n"/>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="3" t="inlineStr">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>פריץ איריס</t>
         </is>
       </c>
-      <c r="B31" s="3" t="inlineStr">
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>19/11</t>
         </is>
       </c>
-      <c r="G31" s="3" t="n"/>
+      <c r="G31" s="2" t="n"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="3" t="inlineStr">
+      <c r="A32" s="2" t="inlineStr">
         <is>
           <t>מרום רותם</t>
         </is>
       </c>
-      <c r="B32" s="3" t="inlineStr">
+      <c r="B32" s="2" t="inlineStr">
         <is>
           <t>22/11</t>
         </is>
       </c>
-      <c r="G32" s="3" t="n"/>
+      <c r="G32" s="2" t="n"/>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="3" t="inlineStr">
+      <c r="A33" s="2" t="inlineStr">
         <is>
           <t>אלון קרן</t>
         </is>
       </c>
-      <c r="B33" s="3" t="inlineStr">
+      <c r="B33" s="2" t="inlineStr">
         <is>
           <t>24/11</t>
         </is>
       </c>
-      <c r="G33" s="3" t="n"/>
+      <c r="G33" s="2" t="n"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="3" t="inlineStr">
+      <c r="A34" s="2" t="inlineStr">
         <is>
           <t>עמור עתליה</t>
         </is>
       </c>
-      <c r="B34" s="3" t="inlineStr">
+      <c r="B34" s="2" t="inlineStr">
         <is>
           <t>29/11</t>
         </is>
       </c>
-      <c r="G34" s="3" t="n"/>
+      <c r="G34" s="2" t="n"/>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="3" t="inlineStr">
+      <c r="A35" s="2" t="inlineStr">
         <is>
           <t>קנמון יעקב</t>
         </is>
       </c>
-      <c r="B35" s="3" t="inlineStr">
+      <c r="B35" s="2" t="inlineStr">
         <is>
           <t>2/12</t>
         </is>
       </c>
-      <c r="G35" s="3" t="n"/>
+      <c r="G35" s="2" t="n"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="3" t="inlineStr">
+      <c r="A36" s="2" t="inlineStr">
         <is>
           <t>שטויק רינה</t>
         </is>
       </c>
-      <c r="B36" s="3" t="inlineStr">
+      <c r="B36" s="2" t="inlineStr">
         <is>
           <t>9/12</t>
         </is>
       </c>
-      <c r="G36" s="3" t="n"/>
+      <c r="G36" s="2" t="n"/>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="3" t="inlineStr">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>כהן ליטל</t>
         </is>
       </c>
-      <c r="B37" s="3" t="inlineStr">
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>11/12</t>
         </is>
       </c>
-      <c r="G37" s="3" t="n"/>
+      <c r="G37" s="2" t="n"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="3" t="inlineStr">
+      <c r="A38" s="2" t="inlineStr">
         <is>
           <t>הנדלמן יפעת</t>
         </is>
       </c>
-      <c r="B38" s="3" t="inlineStr">
+      <c r="B38" s="2" t="inlineStr">
         <is>
           <t>12/12</t>
         </is>
       </c>
-      <c r="G38" s="3" t="n"/>
+      <c r="G38" s="2" t="n"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="3" t="inlineStr">
+      <c r="A39" s="2" t="inlineStr">
         <is>
           <t>חדוות מירית</t>
         </is>
       </c>
-      <c r="B39" s="3" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>14/12</t>
         </is>
       </c>
-      <c r="G39" s="3" t="n"/>
+      <c r="G39" s="2" t="n"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="3" t="inlineStr">
+      <c r="A40" s="2" t="inlineStr">
         <is>
           <t>שיג אמה</t>
         </is>
       </c>
-      <c r="B40" s="3" t="inlineStr">
+      <c r="B40" s="2" t="inlineStr">
         <is>
           <t>14/12</t>
         </is>
       </c>
-      <c r="G40" s="3" t="n"/>
+      <c r="G40" s="2" t="n"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="3" t="inlineStr">
+      <c r="A41" s="2" t="inlineStr">
         <is>
           <t>גראץ אנה</t>
         </is>
       </c>
-      <c r="B41" s="3" t="inlineStr">
+      <c r="B41" s="2" t="inlineStr">
         <is>
           <t>21/12</t>
         </is>
       </c>
-      <c r="G41" s="3" t="n"/>
+      <c r="G41" s="2" t="n"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="3" t="inlineStr">
+      <c r="A42" s="2" t="inlineStr">
         <is>
           <t>בן דוד ענת</t>
         </is>
       </c>
-      <c r="B42" s="3" t="inlineStr">
+      <c r="B42" s="2" t="inlineStr">
         <is>
           <t>23/12</t>
         </is>
       </c>
-      <c r="G42" s="3" t="n"/>
+      <c r="G42" s="2" t="n"/>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="3" t="inlineStr">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>עסיס הילה</t>
         </is>
       </c>
-      <c r="B43" s="3" t="inlineStr">
+      <c r="B43" s="2" t="inlineStr">
         <is>
           <t>24/12</t>
         </is>
       </c>
-      <c r="G43" s="3" t="n"/>
+      <c r="G43" s="2" t="n"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="3" t="inlineStr">
+      <c r="A44" s="2" t="inlineStr">
         <is>
           <t>חכמון סמדר חן</t>
         </is>
       </c>
-      <c r="B44" s="3" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>28/12</t>
         </is>
       </c>
-      <c r="G44" s="3" t="n"/>
+      <c r="G44" s="2" t="n"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
-      <c r="A45" s="3" t="inlineStr">
+      <c r="A45" s="2" t="inlineStr">
         <is>
           <t>דמלין שרית</t>
         </is>
       </c>
-      <c r="B45" s="3" t="inlineStr">
+      <c r="B45" s="2" t="inlineStr">
         <is>
           <t>1/1</t>
         </is>
       </c>
-      <c r="G45" s="3" t="n"/>
+      <c r="G45" s="2" t="n"/>
     </row>
     <row r="46" ht="12.75" customHeight="1">
-      <c r="A46" s="3" t="inlineStr">
+      <c r="A46" s="2" t="inlineStr">
         <is>
           <t>ונונו דבורה</t>
         </is>
       </c>
-      <c r="B46" s="3" t="inlineStr">
+      <c r="B46" s="2" t="inlineStr">
         <is>
           <t>2/1</t>
         </is>
       </c>
-      <c r="G46" s="3" t="n"/>
+      <c r="G46" s="2" t="n"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="3" t="inlineStr">
+      <c r="A47" s="2" t="inlineStr">
         <is>
           <t>פרל ששון רינה</t>
         </is>
       </c>
-      <c r="B47" s="3" t="inlineStr">
+      <c r="B47" s="2" t="inlineStr">
         <is>
           <t>5/1</t>
         </is>
       </c>
-      <c r="G47" s="3" t="n"/>
+      <c r="G47" s="2" t="n"/>
     </row>
     <row r="48" ht="12.75" customHeight="1">
-      <c r="A48" s="3" t="inlineStr">
+      <c r="A48" s="2" t="inlineStr">
         <is>
           <t>טטרסון קארין</t>
         </is>
       </c>
-      <c r="B48" s="3" t="inlineStr">
+      <c r="B48" s="2" t="inlineStr">
         <is>
           <t>5/1</t>
         </is>
       </c>
-      <c r="G48" s="3" t="n"/>
+      <c r="G48" s="2" t="n"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
-      <c r="A49" s="3" t="inlineStr">
+      <c r="A49" s="2" t="inlineStr">
         <is>
           <t>כהן תמי</t>
         </is>
       </c>
-      <c r="B49" s="3" t="inlineStr">
+      <c r="B49" s="2" t="inlineStr">
         <is>
           <t>5/1</t>
         </is>
       </c>
-      <c r="G49" s="3" t="n"/>
+      <c r="G49" s="2" t="n"/>
     </row>
     <row r="50" ht="12.75" customHeight="1">
-      <c r="A50" s="3" t="inlineStr">
+      <c r="A50" s="2" t="inlineStr">
         <is>
           <t>ממן רון</t>
         </is>
       </c>
-      <c r="B50" s="3" t="inlineStr">
+      <c r="B50" s="2" t="inlineStr">
         <is>
           <t>6/1</t>
         </is>
       </c>
-      <c r="G50" s="3" t="n"/>
+      <c r="G50" s="2" t="n"/>
     </row>
     <row r="51" ht="12.75" customHeight="1">
-      <c r="A51" s="3" t="inlineStr">
+      <c r="A51" s="2" t="inlineStr">
         <is>
           <t>אשכנזי רחל</t>
         </is>
       </c>
-      <c r="B51" s="3" t="inlineStr">
+      <c r="B51" s="2" t="inlineStr">
         <is>
           <t>10/1</t>
         </is>
       </c>
-      <c r="G51" s="3" t="n"/>
+      <c r="G51" s="2" t="n"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
-      <c r="A52" s="3" t="inlineStr">
+      <c r="A52" s="2" t="inlineStr">
         <is>
           <t>יחיאל ליעדי</t>
         </is>
       </c>
-      <c r="B52" s="3" t="inlineStr">
+      <c r="B52" s="2" t="inlineStr">
         <is>
           <t>13/1</t>
         </is>
       </c>
-      <c r="G52" s="3" t="n"/>
+      <c r="G52" s="2" t="n"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="3" t="inlineStr">
+      <c r="A53" s="2" t="inlineStr">
         <is>
           <t>איטח עליזה</t>
         </is>
       </c>
-      <c r="B53" s="3" t="inlineStr">
+      <c r="B53" s="2" t="inlineStr">
         <is>
           <t>14/1</t>
         </is>
       </c>
-      <c r="G53" s="3" t="n"/>
+      <c r="G53" s="2" t="n"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="3" t="inlineStr">
+      <c r="A54" s="2" t="inlineStr">
         <is>
           <t>יעקבי בן</t>
         </is>
       </c>
-      <c r="B54" s="3" t="inlineStr">
+      <c r="B54" s="2" t="inlineStr">
         <is>
           <t>19/1</t>
         </is>
       </c>
-      <c r="G54" s="3" t="n"/>
+      <c r="G54" s="2" t="n"/>
     </row>
     <row r="55" ht="12.75" customHeight="1">
-      <c r="A55" s="3" t="inlineStr">
+      <c r="A55" s="2" t="inlineStr">
         <is>
           <t>הרשקוביץ לימור</t>
         </is>
       </c>
-      <c r="B55" s="3" t="inlineStr">
+      <c r="B55" s="2" t="inlineStr">
         <is>
           <t>20/1</t>
         </is>
       </c>
-      <c r="G55" s="3" t="n"/>
+      <c r="G55" s="2" t="n"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" s="3" t="inlineStr">
+      <c r="A56" s="2" t="inlineStr">
         <is>
           <t>ארד חני</t>
         </is>
       </c>
-      <c r="B56" s="3" t="inlineStr">
+      <c r="B56" s="2" t="inlineStr">
         <is>
           <t>20/1</t>
         </is>
       </c>
-      <c r="G56" s="3" t="n"/>
+      <c r="G56" s="2" t="n"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="3" t="inlineStr">
+      <c r="A57" s="2" t="inlineStr">
         <is>
           <t>מגן ישראל</t>
         </is>
       </c>
-      <c r="B57" s="3" t="inlineStr">
+      <c r="B57" s="2" t="inlineStr">
         <is>
           <t>22/1</t>
         </is>
       </c>
-      <c r="G57" s="3" t="n"/>
+      <c r="G57" s="2" t="n"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
-      <c r="A58" s="3" t="inlineStr">
+      <c r="A58" s="2" t="inlineStr">
         <is>
           <t>שפרוני יותם</t>
         </is>
       </c>
-      <c r="B58" s="3" t="inlineStr">
+      <c r="B58" s="2" t="inlineStr">
         <is>
           <t>1/2</t>
         </is>
       </c>
-      <c r="G58" s="3" t="n"/>
+      <c r="G58" s="2" t="n"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
-      <c r="A59" s="3" t="inlineStr">
+      <c r="A59" s="2" t="inlineStr">
         <is>
           <t>בריימן אנה</t>
         </is>
       </c>
-      <c r="B59" s="3" t="inlineStr">
+      <c r="B59" s="2" t="inlineStr">
         <is>
           <t>1/2</t>
         </is>
       </c>
-      <c r="G59" s="3" t="n"/>
+      <c r="G59" s="2" t="n"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
-      <c r="A60" s="3" t="inlineStr">
+      <c r="A60" s="2" t="inlineStr">
         <is>
           <t>חן     יעקב רוסינסקי דליה</t>
         </is>
       </c>
-      <c r="B60" s="3" t="inlineStr">
+      <c r="B60" s="2" t="inlineStr">
         <is>
           <t>11/2</t>
         </is>
       </c>
-      <c r="G60" s="3" t="n"/>
+      <c r="G60" s="2" t="n"/>
     </row>
     <row r="61" ht="12.75" customHeight="1">
-      <c r="A61" s="3" t="inlineStr">
+      <c r="A61" s="2" t="inlineStr">
         <is>
           <t>כהן נועה</t>
         </is>
       </c>
-      <c r="B61" s="3" t="inlineStr">
+      <c r="B61" s="2" t="inlineStr">
         <is>
           <t>12/2</t>
         </is>
       </c>
-      <c r="G61" s="3" t="n"/>
+      <c r="G61" s="2" t="n"/>
     </row>
     <row r="62" ht="12.75" customHeight="1">
-      <c r="A62" s="3" t="inlineStr">
+      <c r="A62" s="2" t="inlineStr">
         <is>
           <t>עובדיה רעות</t>
         </is>
       </c>
-      <c r="B62" s="3" t="inlineStr">
+      <c r="B62" s="2" t="inlineStr">
         <is>
           <t>13/2</t>
         </is>
       </c>
-      <c r="G62" s="3" t="n"/>
+      <c r="G62" s="2" t="n"/>
     </row>
     <row r="63" ht="12.75" customHeight="1">
-      <c r="A63" s="3" t="inlineStr">
+      <c r="A63" s="2" t="inlineStr">
         <is>
           <t>פרבר אירית</t>
         </is>
       </c>
-      <c r="B63" s="3" t="inlineStr">
+      <c r="B63" s="2" t="inlineStr">
         <is>
           <t>14/2</t>
         </is>
       </c>
-      <c r="G63" s="3" t="n"/>
+      <c r="G63" s="2" t="n"/>
     </row>
     <row r="64" ht="12.75" customHeight="1">
-      <c r="A64" s="3" t="inlineStr">
+      <c r="A64" s="2" t="inlineStr">
         <is>
           <t>נבו יעקב</t>
         </is>
       </c>
-      <c r="B64" s="3" t="inlineStr">
+      <c r="B64" s="2" t="inlineStr">
         <is>
           <t>18/2</t>
         </is>
       </c>
-      <c r="G64" s="3" t="n"/>
+      <c r="G64" s="2" t="n"/>
     </row>
     <row r="65" ht="12.75" customHeight="1">
-      <c r="A65" s="3" t="inlineStr">
+      <c r="A65" s="2" t="inlineStr">
         <is>
           <t>מירב אור</t>
         </is>
       </c>
-      <c r="B65" s="3" t="inlineStr">
+      <c r="B65" s="2" t="inlineStr">
         <is>
           <t>22/2</t>
         </is>
       </c>
-      <c r="G65" s="3" t="n"/>
+      <c r="G65" s="2" t="n"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
-      <c r="A66" s="3" t="inlineStr">
+      <c r="A66" s="2" t="inlineStr">
         <is>
           <t>צרור גלית</t>
         </is>
       </c>
-      <c r="B66" s="3" t="inlineStr">
+      <c r="B66" s="2" t="inlineStr">
         <is>
           <t>22/2</t>
         </is>
       </c>
-      <c r="G66" s="3" t="n"/>
+      <c r="G66" s="2" t="n"/>
     </row>
     <row r="67" ht="12.75" customHeight="1">
-      <c r="A67" s="3" t="inlineStr">
+      <c r="A67" s="2" t="inlineStr">
         <is>
           <t>לנדאו גיל</t>
         </is>
       </c>
-      <c r="B67" s="3" t="inlineStr">
+      <c r="B67" s="2" t="inlineStr">
         <is>
           <t>23/2</t>
         </is>
       </c>
-      <c r="G67" s="3" t="n"/>
+      <c r="G67" s="2" t="n"/>
     </row>
     <row r="68" ht="12.75" customHeight="1">
-      <c r="A68" s="3" t="inlineStr">
+      <c r="A68" s="2" t="inlineStr">
         <is>
           <t>סלע רמה</t>
         </is>
       </c>
-      <c r="B68" s="3" t="inlineStr">
+      <c r="B68" s="2" t="inlineStr">
         <is>
           <t>27/2</t>
         </is>
       </c>
-      <c r="G68" s="3" t="n"/>
+      <c r="G68" s="2" t="n"/>
     </row>
     <row r="69" ht="12.75" customHeight="1">
-      <c r="A69" s="3" t="inlineStr">
+      <c r="A69" s="2" t="inlineStr">
         <is>
           <t>ואנונו שלום</t>
         </is>
       </c>
-      <c r="B69" s="3" t="inlineStr">
+      <c r="B69" s="2" t="inlineStr">
         <is>
           <t>27/2</t>
         </is>
       </c>
-      <c r="G69" s="3" t="n"/>
+      <c r="G69" s="2" t="n"/>
     </row>
     <row r="70" ht="12.75" customHeight="1">
-      <c r="A70" s="3" t="inlineStr">
+      <c r="A70" s="2" t="inlineStr">
         <is>
           <t>גרונברג כהן מלינה יעל</t>
         </is>
       </c>
-      <c r="B70" s="3" t="inlineStr">
+      <c r="B70" s="2" t="inlineStr">
         <is>
           <t>27/2</t>
         </is>
       </c>
-      <c r="G70" s="3" t="n"/>
+      <c r="G70" s="2" t="n"/>
     </row>
     <row r="71" ht="12.75" customHeight="1">
-      <c r="A71" s="3" t="inlineStr">
+      <c r="A71" s="2" t="inlineStr">
         <is>
           <t>שחר עדן</t>
         </is>
       </c>
-      <c r="B71" s="3" t="inlineStr">
+      <c r="B71" s="2" t="inlineStr">
         <is>
           <t>3/3</t>
         </is>
       </c>
-      <c r="G71" s="3" t="n"/>
+      <c r="G71" s="2" t="n"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
-      <c r="A72" s="3" t="inlineStr">
+      <c r="A72" s="2" t="inlineStr">
         <is>
           <t>שווץ גילה</t>
         </is>
       </c>
-      <c r="B72" s="3" t="inlineStr">
+      <c r="B72" s="2" t="inlineStr">
         <is>
           <t>4/3</t>
         </is>
       </c>
-      <c r="G72" s="3" t="n"/>
+      <c r="G72" s="2" t="n"/>
     </row>
     <row r="73" ht="12.75" customHeight="1">
-      <c r="A73" s="3" t="inlineStr">
+      <c r="A73" s="2" t="inlineStr">
         <is>
           <t>גולדשטיין הררי דנה</t>
         </is>
       </c>
-      <c r="B73" s="3" t="inlineStr">
+      <c r="B73" s="2" t="inlineStr">
         <is>
           <t>5/3</t>
         </is>
       </c>
-      <c r="G73" s="3" t="n"/>
+      <c r="G73" s="2" t="n"/>
     </row>
     <row r="74" ht="12.75" customHeight="1">
-      <c r="A74" s="3" t="inlineStr">
+      <c r="A74" s="2" t="inlineStr">
         <is>
           <t>שרון קליין מעיין</t>
         </is>
       </c>
-      <c r="B74" s="3" t="inlineStr">
+      <c r="B74" s="2" t="inlineStr">
         <is>
           <t>14/3</t>
         </is>
       </c>
-      <c r="G74" s="3" t="n"/>
+      <c r="G74" s="2" t="n"/>
     </row>
     <row r="75" ht="12.75" customHeight="1">
-      <c r="A75" s="3" t="inlineStr">
+      <c r="A75" s="2" t="inlineStr">
         <is>
           <t>פלצמן בל יפה</t>
         </is>
       </c>
-      <c r="B75" s="3" t="inlineStr">
+      <c r="B75" s="2" t="inlineStr">
         <is>
           <t>15/3</t>
         </is>
       </c>
-      <c r="G75" s="3" t="n"/>
+      <c r="G75" s="2" t="n"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
-      <c r="A76" s="3" t="inlineStr">
+      <c r="A76" s="2" t="inlineStr">
         <is>
           <t>אביעוז מזל</t>
         </is>
       </c>
-      <c r="B76" s="3" t="inlineStr">
+      <c r="B76" s="2" t="inlineStr">
         <is>
           <t>22/3</t>
         </is>
       </c>
-      <c r="G76" s="3" t="n"/>
+      <c r="G76" s="2" t="n"/>
     </row>
     <row r="77" ht="12.75" customHeight="1">
-      <c r="A77" s="3" t="inlineStr">
+      <c r="A77" s="2" t="inlineStr">
         <is>
           <t>טרובניאקוב אילנה</t>
         </is>
       </c>
-      <c r="B77" s="3" t="inlineStr">
+      <c r="B77" s="2" t="inlineStr">
         <is>
           <t>25/3</t>
         </is>
       </c>
-      <c r="G77" s="3" t="n"/>
+      <c r="G77" s="2" t="n"/>
     </row>
     <row r="78" ht="12.75" customHeight="1">
-      <c r="A78" s="3" t="inlineStr">
+      <c r="A78" s="2" t="inlineStr">
         <is>
           <t>לוינסון אייל עדי</t>
         </is>
       </c>
-      <c r="B78" s="3" t="inlineStr">
+      <c r="B78" s="2" t="inlineStr">
         <is>
           <t>27/3</t>
         </is>
       </c>
-      <c r="G78" s="3" t="n"/>
+      <c r="G78" s="2" t="n"/>
     </row>
     <row r="79" ht="12.75" customHeight="1">
-      <c r="A79" s="3" t="inlineStr">
+      <c r="A79" s="2" t="inlineStr">
         <is>
           <t>וולפסון משה יצחק</t>
         </is>
       </c>
-      <c r="B79" s="3" t="inlineStr">
+      <c r="B79" s="2" t="inlineStr">
         <is>
           <t>28/3</t>
         </is>
       </c>
-      <c r="G79" s="3" t="n"/>
+      <c r="G79" s="2" t="n"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
-      <c r="A80" s="3" t="inlineStr">
+      <c r="A80" s="2" t="inlineStr">
         <is>
           <t>גוטוירט ורד</t>
         </is>
       </c>
-      <c r="B80" s="3" t="inlineStr">
+      <c r="B80" s="2" t="inlineStr">
         <is>
           <t>6/4</t>
         </is>
       </c>
-      <c r="G80" s="3" t="n"/>
+      <c r="G80" s="2" t="n"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
-      <c r="A81" s="3" t="inlineStr">
+      <c r="A81" s="2" t="inlineStr">
         <is>
           <t>כהן ענבל</t>
         </is>
       </c>
-      <c r="B81" s="3" t="inlineStr">
+      <c r="B81" s="2" t="inlineStr">
         <is>
           <t>12/4</t>
         </is>
       </c>
-      <c r="G81" s="3" t="n"/>
+      <c r="G81" s="2" t="n"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
-      <c r="A82" s="3" t="inlineStr">
+      <c r="A82" s="2" t="inlineStr">
         <is>
           <t>גבאי אסתר</t>
         </is>
       </c>
-      <c r="B82" s="3" t="inlineStr">
+      <c r="B82" s="2" t="inlineStr">
         <is>
           <t>16/4</t>
         </is>
       </c>
-      <c r="G82" s="3" t="n"/>
+      <c r="G82" s="2" t="n"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
-      <c r="A83" s="3" t="inlineStr">
+      <c r="A83" s="2" t="inlineStr">
         <is>
           <t>דלל ציפי</t>
         </is>
       </c>
-      <c r="B83" s="3" t="inlineStr">
+      <c r="B83" s="2" t="inlineStr">
         <is>
           <t>19/4</t>
         </is>
       </c>
-      <c r="G83" s="3" t="n"/>
+      <c r="G83" s="2" t="n"/>
     </row>
     <row r="84" ht="12.75" customHeight="1">
-      <c r="A84" s="3" t="inlineStr">
+      <c r="A84" s="2" t="inlineStr">
         <is>
           <t>אוזדנה מרי</t>
         </is>
       </c>
-      <c r="B84" s="3" t="inlineStr">
+      <c r="B84" s="2" t="inlineStr">
         <is>
           <t>19/4</t>
         </is>
       </c>
-      <c r="G84" s="3" t="n"/>
+      <c r="G84" s="2" t="n"/>
     </row>
     <row r="85" ht="12.75" customHeight="1">
-      <c r="A85" s="3" t="inlineStr">
+      <c r="A85" s="2" t="inlineStr">
         <is>
           <t>ריכליס מרים</t>
         </is>
       </c>
-      <c r="B85" s="3" t="inlineStr">
+      <c r="B85" s="2" t="inlineStr">
         <is>
           <t>20/4</t>
         </is>
       </c>
-      <c r="G85" s="3" t="n"/>
+      <c r="G85" s="2" t="n"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
-      <c r="A86" s="3" t="inlineStr">
+      <c r="A86" s="2" t="inlineStr">
         <is>
           <t>אטלסמן דרורית</t>
         </is>
       </c>
-      <c r="B86" s="3" t="inlineStr">
+      <c r="B86" s="2" t="inlineStr">
         <is>
           <t>20/4</t>
         </is>
       </c>
-      <c r="G86" s="3" t="n"/>
+      <c r="G86" s="2" t="n"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
-      <c r="A87" s="3" t="inlineStr">
+      <c r="A87" s="2" t="inlineStr">
         <is>
           <t>ברנר אבי</t>
         </is>
       </c>
-      <c r="B87" s="3" t="inlineStr">
+      <c r="B87" s="2" t="inlineStr">
         <is>
           <t>21/4</t>
         </is>
       </c>
-      <c r="G87" s="3" t="n"/>
+      <c r="G87" s="2" t="n"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
-      <c r="A88" s="3" t="inlineStr">
+      <c r="A88" s="2" t="inlineStr">
         <is>
           <t>המדאני כהן שירה</t>
         </is>
       </c>
-      <c r="B88" s="3" t="inlineStr">
+      <c r="B88" s="2" t="inlineStr">
         <is>
           <t>21/4</t>
         </is>
       </c>
-      <c r="G88" s="3" t="n"/>
+      <c r="G88" s="2" t="n"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
-      <c r="A89" s="3" t="inlineStr">
+      <c r="A89" s="2" t="inlineStr">
         <is>
           <t>שרעבי דלית</t>
         </is>
       </c>
-      <c r="B89" s="3" t="inlineStr">
+      <c r="B89" s="2" t="inlineStr">
         <is>
           <t>22/4</t>
         </is>
       </c>
-      <c r="G89" s="3" t="n"/>
+      <c r="G89" s="2" t="n"/>
     </row>
     <row r="90" ht="12.75" customHeight="1">
-      <c r="A90" s="3" t="inlineStr">
+      <c r="A90" s="2" t="inlineStr">
         <is>
           <t>עומסי מיכל</t>
         </is>
       </c>
-      <c r="B90" s="3" t="inlineStr">
+      <c r="B90" s="2" t="inlineStr">
         <is>
           <t>24/4</t>
         </is>
       </c>
-      <c r="G90" s="3" t="n"/>
+      <c r="G90" s="2" t="n"/>
     </row>
     <row r="91" ht="12.75" customHeight="1">
-      <c r="A91" s="3" t="inlineStr">
+      <c r="A91" s="2" t="inlineStr">
         <is>
           <t>גלילי עסיס ורדה</t>
         </is>
       </c>
-      <c r="B91" s="3" t="inlineStr">
+      <c r="B91" s="2" t="inlineStr">
         <is>
           <t>25/4</t>
         </is>
       </c>
-      <c r="G91" s="3" t="n"/>
+      <c r="G91" s="2" t="n"/>
     </row>
     <row r="92" ht="12.75" customHeight="1">
-      <c r="A92" s="3" t="inlineStr">
+      <c r="A92" s="2" t="inlineStr">
         <is>
           <t>כהן באר ענת</t>
         </is>
       </c>
-      <c r="B92" s="3" t="inlineStr">
+      <c r="B92" s="2" t="inlineStr">
         <is>
           <t>30/4</t>
         </is>
       </c>
-      <c r="G92" s="3" t="n"/>
+      <c r="G92" s="2" t="n"/>
     </row>
     <row r="93" ht="12.75" customHeight="1">
-      <c r="A93" s="3" t="inlineStr">
+      <c r="A93" s="2" t="inlineStr">
         <is>
           <t>מויאל שלמה</t>
         </is>
       </c>
-      <c r="B93" s="3" t="inlineStr">
+      <c r="B93" s="2" t="inlineStr">
         <is>
           <t>1/5</t>
         </is>
       </c>
-      <c r="G93" s="3" t="n"/>
+      <c r="G93" s="2" t="n"/>
     </row>
     <row r="94" ht="12.75" customHeight="1">
-      <c r="A94" s="3" t="inlineStr">
+      <c r="A94" s="2" t="inlineStr">
         <is>
           <t>גודניאן לינוי</t>
         </is>
       </c>
-      <c r="B94" s="3" t="inlineStr">
+      <c r="B94" s="2" t="inlineStr">
         <is>
           <t>1/5</t>
         </is>
       </c>
-      <c r="G94" s="3" t="n"/>
+      <c r="G94" s="2" t="n"/>
     </row>
     <row r="95" ht="12.75" customHeight="1">
-      <c r="A95" s="3" t="inlineStr">
+      <c r="A95" s="2" t="inlineStr">
         <is>
           <t>ידיד גלעד</t>
         </is>
       </c>
-      <c r="B95" s="3" t="inlineStr">
+      <c r="B95" s="2" t="inlineStr">
         <is>
           <t>1/5</t>
         </is>
       </c>
-      <c r="G95" s="3" t="n"/>
+      <c r="G95" s="2" t="n"/>
     </row>
     <row r="96" ht="12.75" customHeight="1">
-      <c r="A96" s="3" t="inlineStr">
+      <c r="A96" s="2" t="inlineStr">
         <is>
           <t>דורון איריס</t>
         </is>
       </c>
-      <c r="B96" s="3" t="inlineStr">
+      <c r="B96" s="2" t="inlineStr">
         <is>
           <t>5/5</t>
         </is>
       </c>
-      <c r="G96" s="3" t="n"/>
+      <c r="G96" s="2" t="n"/>
     </row>
     <row r="97" ht="12.75" customHeight="1">
-      <c r="A97" s="3" t="inlineStr">
+      <c r="A97" s="2" t="inlineStr">
         <is>
           <t>קגן רבקה</t>
         </is>
       </c>
-      <c r="B97" s="3" t="inlineStr">
+      <c r="B97" s="2" t="inlineStr">
         <is>
           <t>10/5</t>
         </is>
       </c>
-      <c r="G97" s="3" t="n"/>
+      <c r="G97" s="2" t="n"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
-      <c r="A98" s="3" t="inlineStr">
+      <c r="A98" s="2" t="inlineStr">
         <is>
           <t>כלפון ברקובי רונית</t>
         </is>
       </c>
-      <c r="B98" s="3" t="inlineStr">
+      <c r="B98" s="2" t="inlineStr">
         <is>
           <t>11/5</t>
         </is>
       </c>
-      <c r="G98" s="3" t="n"/>
+      <c r="G98" s="2" t="n"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
-      <c r="A99" s="3" t="inlineStr">
+      <c r="A99" s="2" t="inlineStr">
         <is>
           <t>זליקוביץ איריס</t>
         </is>
       </c>
-      <c r="B99" s="3" t="inlineStr">
+      <c r="B99" s="2" t="inlineStr">
         <is>
           <t>13/5</t>
         </is>
       </c>
-      <c r="G99" s="3" t="n"/>
+      <c r="G99" s="2" t="n"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
-      <c r="A100" s="3" t="inlineStr">
+      <c r="A100" s="2" t="inlineStr">
         <is>
           <t>כהן מנחם</t>
         </is>
       </c>
-      <c r="B100" s="3" t="inlineStr">
+      <c r="B100" s="2" t="inlineStr">
         <is>
           <t>15/5</t>
         </is>
       </c>
-      <c r="G100" s="3" t="n"/>
+      <c r="G100" s="2" t="n"/>
     </row>
     <row r="101" ht="12.75" customHeight="1">
-      <c r="A101" s="3" t="inlineStr">
+      <c r="A101" s="2" t="inlineStr">
         <is>
           <t>שריון רונית</t>
         </is>
       </c>
-      <c r="B101" s="3" t="inlineStr">
+      <c r="B101" s="2" t="inlineStr">
         <is>
           <t>17/5</t>
         </is>
       </c>
-      <c r="G101" s="3" t="n"/>
+      <c r="G101" s="2" t="n"/>
     </row>
     <row r="102" ht="12.75" customHeight="1">
-      <c r="A102" s="3" t="inlineStr">
+      <c r="A102" s="2" t="inlineStr">
         <is>
           <t>שלו אורי</t>
         </is>
       </c>
-      <c r="B102" s="3" t="inlineStr">
+      <c r="B102" s="2" t="inlineStr">
         <is>
           <t>17/5</t>
         </is>
       </c>
-      <c r="G102" s="3" t="n"/>
+      <c r="G102" s="2" t="n"/>
     </row>
     <row r="103" ht="12.75" customHeight="1">
-      <c r="A103" s="3" t="inlineStr">
+      <c r="A103" s="2" t="inlineStr">
         <is>
           <t>קדוש גל</t>
         </is>
       </c>
-      <c r="B103" s="3" t="inlineStr">
+      <c r="B103" s="2" t="inlineStr">
         <is>
           <t>19/5</t>
         </is>
       </c>
-      <c r="G103" s="3" t="n"/>
+      <c r="G103" s="2" t="n"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
-      <c r="A104" s="3" t="inlineStr">
+      <c r="A104" s="2" t="inlineStr">
         <is>
           <t>מנדל קרינה</t>
         </is>
       </c>
-      <c r="B104" s="3" t="inlineStr">
+      <c r="B104" s="2" t="inlineStr">
         <is>
           <t>20/5</t>
         </is>
       </c>
-      <c r="G104" s="3" t="n"/>
+      <c r="G104" s="2" t="n"/>
     </row>
     <row r="105" ht="12.75" customHeight="1">
-      <c r="A105" s="3" t="inlineStr">
+      <c r="A105" s="2" t="inlineStr">
         <is>
           <t>אילוז חן</t>
         </is>
       </c>
-      <c r="B105" s="3" t="inlineStr">
+      <c r="B105" s="2" t="inlineStr">
         <is>
           <t>20/5</t>
         </is>
       </c>
-      <c r="G105" s="3" t="n"/>
+      <c r="G105" s="2" t="n"/>
     </row>
     <row r="106" ht="12.75" customHeight="1">
-      <c r="A106" s="3" t="inlineStr">
+      <c r="A106" s="2" t="inlineStr">
         <is>
           <t>חייט מיכל</t>
         </is>
       </c>
-      <c r="B106" s="3" t="inlineStr">
+      <c r="B106" s="2" t="inlineStr">
         <is>
           <t>22/5</t>
         </is>
       </c>
-      <c r="G106" s="3" t="n"/>
+      <c r="G106" s="2" t="n"/>
     </row>
     <row r="107" ht="12.75" customHeight="1">
-      <c r="A107" s="3" t="inlineStr">
+      <c r="A107" s="2" t="inlineStr">
         <is>
           <t>ציפר איילת</t>
         </is>
       </c>
-      <c r="B107" s="3" t="inlineStr">
+      <c r="B107" s="2" t="inlineStr">
         <is>
           <t>2/6</t>
         </is>
       </c>
-      <c r="G107" s="3" t="n"/>
+      <c r="G107" s="2" t="n"/>
     </row>
     <row r="108" ht="12.75" customHeight="1">
-      <c r="A108" s="3" t="inlineStr">
+      <c r="A108" s="2" t="inlineStr">
         <is>
           <t>רם הילה</t>
         </is>
       </c>
-      <c r="B108" s="3" t="inlineStr">
+      <c r="B108" s="2" t="inlineStr">
         <is>
           <t>2/6</t>
         </is>
       </c>
-      <c r="G108" s="3" t="n"/>
+      <c r="G108" s="2" t="n"/>
     </row>
     <row r="109" ht="12.75" customHeight="1">
-      <c r="A109" s="3" t="inlineStr">
+      <c r="A109" s="2" t="inlineStr">
         <is>
           <t>רז רחל</t>
         </is>
       </c>
-      <c r="B109" s="3" t="inlineStr">
+      <c r="B109" s="2" t="inlineStr">
         <is>
           <t>4/6</t>
         </is>
       </c>
-      <c r="G109" s="3" t="n"/>
+      <c r="G109" s="2" t="n"/>
     </row>
     <row r="110" ht="12.75" customHeight="1">
-      <c r="A110" s="3" t="inlineStr">
+      <c r="A110" s="2" t="inlineStr">
         <is>
           <t>יאנובסקי-ציגנוק אנה</t>
         </is>
       </c>
-      <c r="B110" s="3" t="inlineStr">
+      <c r="B110" s="2" t="inlineStr">
         <is>
           <t>6/6</t>
         </is>
       </c>
-      <c r="G110" s="3" t="n"/>
+      <c r="G110" s="2" t="n"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
-      <c r="A111" s="3" t="inlineStr">
+      <c r="A111" s="2" t="inlineStr">
         <is>
           <t>יוספי יורם</t>
         </is>
       </c>
-      <c r="B111" s="3" t="inlineStr">
+      <c r="B111" s="2" t="inlineStr">
         <is>
           <t>8/6</t>
         </is>
       </c>
-      <c r="G111" s="3" t="n"/>
+      <c r="G111" s="2" t="n"/>
     </row>
     <row r="112" ht="12.75" customHeight="1">
-      <c r="A112" s="3" t="inlineStr">
+      <c r="A112" s="2" t="inlineStr">
         <is>
           <t>הכלר ברוך</t>
         </is>
       </c>
-      <c r="B112" s="3" t="inlineStr">
+      <c r="B112" s="2" t="inlineStr">
         <is>
           <t>9/6</t>
         </is>
       </c>
-      <c r="G112" s="3" t="n"/>
+      <c r="G112" s="2" t="n"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
-      <c r="A113" s="3" t="inlineStr">
+      <c r="A113" s="2" t="inlineStr">
         <is>
           <t>ברון אריק</t>
         </is>
       </c>
-      <c r="B113" s="3" t="inlineStr">
+      <c r="B113" s="2" t="inlineStr">
         <is>
           <t>9/6</t>
         </is>
       </c>
-      <c r="G113" s="3" t="n"/>
+      <c r="G113" s="2" t="n"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
-      <c r="A114" s="3" t="inlineStr">
+      <c r="A114" s="2" t="inlineStr">
         <is>
           <t>קנדבי אילנה</t>
         </is>
       </c>
-      <c r="B114" s="3" t="inlineStr">
+      <c r="B114" s="2" t="inlineStr">
         <is>
           <t>10/6</t>
         </is>
       </c>
-      <c r="G114" s="3" t="n"/>
+      <c r="G114" s="2" t="n"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
-      <c r="A115" s="3" t="inlineStr">
+      <c r="A115" s="2" t="inlineStr">
         <is>
           <t>מזרחי עדי</t>
         </is>
       </c>
-      <c r="B115" s="3" t="inlineStr">
+      <c r="B115" s="2" t="inlineStr">
         <is>
           <t>11/6</t>
         </is>
       </c>
-      <c r="G115" s="3" t="n"/>
+      <c r="G115" s="2" t="n"/>
     </row>
     <row r="116" ht="12.75" customHeight="1">
-      <c r="A116" s="3" t="inlineStr">
+      <c r="A116" s="2" t="inlineStr">
         <is>
           <t>בן נון טל</t>
         </is>
       </c>
-      <c r="B116" s="3" t="inlineStr">
+      <c r="B116" s="2" t="inlineStr">
         <is>
           <t>12/6</t>
         </is>
       </c>
-      <c r="G116" s="3" t="n"/>
+      <c r="G116" s="2" t="n"/>
     </row>
     <row r="117" ht="12.75" customHeight="1">
-      <c r="A117" s="3" t="inlineStr">
+      <c r="A117" s="2" t="inlineStr">
         <is>
           <t>שרעבי רותם</t>
         </is>
       </c>
-      <c r="B117" s="3" t="inlineStr">
+      <c r="B117" s="2" t="inlineStr">
         <is>
           <t>14/6</t>
         </is>
       </c>
-      <c r="G117" s="3" t="n"/>
+      <c r="G117" s="2" t="n"/>
     </row>
     <row r="118" ht="12.75" customHeight="1">
-      <c r="A118" s="3" t="inlineStr">
+      <c r="A118" s="2" t="inlineStr">
         <is>
           <t>צור יהודית</t>
         </is>
       </c>
-      <c r="B118" s="3" t="inlineStr">
+      <c r="B118" s="2" t="inlineStr">
         <is>
           <t>15/6</t>
         </is>
       </c>
-      <c r="G118" s="3" t="n"/>
+      <c r="G118" s="2" t="n"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
-      <c r="A119" s="3" t="inlineStr">
+      <c r="A119" s="2" t="inlineStr">
         <is>
           <t>אבורמדן אמנה</t>
         </is>
       </c>
-      <c r="B119" s="3" t="inlineStr">
+      <c r="B119" s="2" t="inlineStr">
         <is>
           <t>18/6</t>
         </is>
       </c>
-      <c r="G119" s="3" t="n"/>
+      <c r="G119" s="2" t="n"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
-      <c r="A120" s="3" t="inlineStr">
+      <c r="A120" s="2" t="inlineStr">
         <is>
           <t>דקל יהודית</t>
         </is>
       </c>
-      <c r="B120" s="3" t="inlineStr">
+      <c r="B120" s="2" t="inlineStr">
         <is>
           <t>26/6</t>
         </is>
       </c>
-      <c r="G120" s="3" t="n"/>
+      <c r="G120" s="2" t="n"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
-      <c r="A121" s="3" t="inlineStr">
+      <c r="A121" s="2" t="inlineStr">
         <is>
           <t>מזור רחלי</t>
         </is>
       </c>
-      <c r="B121" s="3" t="inlineStr">
+      <c r="B121" s="2" t="inlineStr">
         <is>
           <t>29/6</t>
         </is>
       </c>
-      <c r="G121" s="3" t="n"/>
+      <c r="G121" s="2" t="n"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
-      <c r="A122" s="3" t="inlineStr">
+      <c r="A122" s="2" t="inlineStr">
         <is>
           <t>מנשה הילה</t>
         </is>
       </c>
-      <c r="B122" s="3" t="inlineStr">
+      <c r="B122" s="2" t="inlineStr">
         <is>
           <t>30/6</t>
         </is>
       </c>
-      <c r="G122" s="3" t="n"/>
+      <c r="G122" s="2" t="n"/>
     </row>
     <row r="123" ht="12.75" customHeight="1">
-      <c r="A123" s="3" t="inlineStr">
+      <c r="A123" s="2" t="inlineStr">
         <is>
           <t>זלצמן מיכל</t>
         </is>
       </c>
-      <c r="B123" s="3" t="inlineStr">
+      <c r="B123" s="2" t="inlineStr">
         <is>
           <t>2/7</t>
         </is>
       </c>
-      <c r="G123" s="3" t="n"/>
+      <c r="G123" s="2" t="n"/>
     </row>
     <row r="124" ht="12.75" customHeight="1">
-      <c r="A124" s="3" t="inlineStr">
+      <c r="A124" s="2" t="inlineStr">
         <is>
           <t>מטרינסקי יקטרינה</t>
         </is>
       </c>
-      <c r="B124" s="3" t="inlineStr">
+      <c r="B124" s="2" t="inlineStr">
         <is>
           <t>4/7</t>
         </is>
       </c>
-      <c r="G124" s="3" t="n"/>
+      <c r="G124" s="2" t="n"/>
     </row>
     <row r="125" ht="12.75" customHeight="1">
-      <c r="A125" s="3" t="inlineStr">
+      <c r="A125" s="2" t="inlineStr">
         <is>
           <t>איליאשנקו קונסטנטי</t>
         </is>
       </c>
-      <c r="B125" s="3" t="inlineStr">
+      <c r="B125" s="2" t="inlineStr">
         <is>
           <t>5/7</t>
         </is>
       </c>
-      <c r="G125" s="3" t="n"/>
+      <c r="G125" s="2" t="n"/>
     </row>
     <row r="126" ht="12.75" customHeight="1">
-      <c r="A126" s="3" t="inlineStr">
+      <c r="A126" s="2" t="inlineStr">
         <is>
           <t>קוריאט דניאלה</t>
         </is>
       </c>
-      <c r="B126" s="3" t="inlineStr">
+      <c r="B126" s="2" t="inlineStr">
         <is>
           <t>6/7</t>
         </is>
       </c>
-      <c r="G126" s="3" t="n"/>
+      <c r="G126" s="2" t="n"/>
     </row>
     <row r="127" ht="12.75" customHeight="1">
-      <c r="A127" s="3" t="inlineStr">
+      <c r="A127" s="2" t="inlineStr">
         <is>
           <t>פרח שבלי</t>
         </is>
       </c>
-      <c r="B127" s="3" t="inlineStr">
+      <c r="B127" s="2" t="inlineStr">
         <is>
           <t>11/7</t>
         </is>
       </c>
-      <c r="G127" s="3" t="n"/>
+      <c r="G127" s="2" t="n"/>
     </row>
     <row r="128" ht="12.75" customHeight="1">
-      <c r="A128" s="3" t="inlineStr">
+      <c r="A128" s="2" t="inlineStr">
         <is>
           <t>כהן קורל</t>
         </is>
       </c>
-      <c r="B128" s="3" t="inlineStr">
+      <c r="B128" s="2" t="inlineStr">
         <is>
           <t>13/7</t>
         </is>
       </c>
-      <c r="G128" s="3" t="n"/>
+      <c r="G128" s="2" t="n"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
-      <c r="A129" s="3" t="inlineStr">
+      <c r="A129" s="2" t="inlineStr">
         <is>
           <t>קוסקס-סנגור אורלי</t>
         </is>
       </c>
-      <c r="B129" s="3" t="inlineStr">
+      <c r="B129" s="2" t="inlineStr">
         <is>
           <t>17/7</t>
         </is>
       </c>
-      <c r="G129" s="3" t="n"/>
+      <c r="G129" s="2" t="n"/>
     </row>
     <row r="130" ht="12.75" customHeight="1">
-      <c r="A130" s="3" t="inlineStr">
+      <c r="A130" s="2" t="inlineStr">
         <is>
           <t>פרשל שיראל</t>
         </is>
       </c>
-      <c r="B130" s="3" t="inlineStr">
+      <c r="B130" s="2" t="inlineStr">
         <is>
           <t>21/7</t>
         </is>
       </c>
-      <c r="G130" s="3" t="n"/>
+      <c r="G130" s="2" t="n"/>
     </row>
     <row r="131" ht="12.75" customHeight="1">
-      <c r="A131" s="3" t="inlineStr">
+      <c r="A131" s="2" t="inlineStr">
         <is>
           <t>ימין חגית</t>
         </is>
       </c>
-      <c r="B131" s="3" t="inlineStr">
+      <c r="B131" s="2" t="inlineStr">
         <is>
           <t>24/7</t>
         </is>
       </c>
-      <c r="G131" s="3" t="n"/>
+      <c r="G131" s="2" t="n"/>
     </row>
     <row r="132" ht="12.75" customHeight="1">
-      <c r="A132" s="3" t="inlineStr">
+      <c r="A132" s="2" t="inlineStr">
         <is>
           <t>חדד מיטל</t>
         </is>
       </c>
-      <c r="B132" s="3" t="inlineStr">
+      <c r="B132" s="2" t="inlineStr">
         <is>
           <t>25/7</t>
         </is>
       </c>
-      <c r="G132" s="3" t="n"/>
+      <c r="G132" s="2" t="n"/>
     </row>
     <row r="133" ht="12.75" customHeight="1">
-      <c r="A133" s="3" t="inlineStr">
+      <c r="A133" s="2" t="inlineStr">
         <is>
           <t>שפירא נילי</t>
         </is>
       </c>
-      <c r="B133" s="3" t="inlineStr">
+      <c r="B133" s="2" t="inlineStr">
         <is>
           <t>27/7</t>
         </is>
       </c>
-      <c r="G133" s="3" t="n"/>
+      <c r="G133" s="2" t="n"/>
     </row>
     <row r="134" ht="12.75" customHeight="1">
-      <c r="A134" s="3" t="inlineStr">
+      <c r="A134" s="2" t="inlineStr">
         <is>
           <t>טייב אולגה</t>
         </is>
       </c>
-      <c r="B134" s="3" t="inlineStr">
+      <c r="B134" s="2" t="inlineStr">
         <is>
           <t>31/7</t>
         </is>
       </c>
-      <c r="G134" s="3" t="n"/>
+      <c r="G134" s="2" t="n"/>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="3" t="inlineStr">
+      <c r="A135" s="2" t="inlineStr">
         <is>
           <t>רבינוביץ מרינה</t>
         </is>
       </c>
-      <c r="B135" s="3" t="inlineStr">
+      <c r="B135" s="2" t="inlineStr">
         <is>
           <t>3/8</t>
         </is>
       </c>
-      <c r="G135" s="3" t="n"/>
+      <c r="G135" s="2" t="n"/>
     </row>
     <row r="136" ht="12.75" customHeight="1">
-      <c r="A136" s="3" t="inlineStr">
+      <c r="A136" s="2" t="inlineStr">
         <is>
           <t>גוטפלד רונית</t>
         </is>
       </c>
-      <c r="B136" s="3" t="inlineStr">
+      <c r="B136" s="2" t="inlineStr">
         <is>
           <t>4/8</t>
         </is>
       </c>
-      <c r="G136" s="3" t="n"/>
+      <c r="G136" s="2" t="n"/>
     </row>
     <row r="137" ht="12.75" customHeight="1">
-      <c r="A137" s="3" t="inlineStr">
+      <c r="A137" s="2" t="inlineStr">
         <is>
           <t>כרמי נגה</t>
         </is>
       </c>
-      <c r="B137" s="3" t="inlineStr">
+      <c r="B137" s="2" t="inlineStr">
         <is>
           <t>7/8</t>
         </is>
       </c>
-      <c r="G137" s="3" t="n"/>
+      <c r="G137" s="2" t="n"/>
     </row>
     <row r="138" ht="12.75" customHeight="1">
-      <c r="A138" s="3" t="inlineStr">
+      <c r="A138" s="2" t="inlineStr">
         <is>
           <t>אוברשטיין אדוה</t>
         </is>
       </c>
-      <c r="B138" s="3" t="inlineStr">
+      <c r="B138" s="2" t="inlineStr">
         <is>
           <t>8/8</t>
         </is>
       </c>
-      <c r="G138" s="3" t="n"/>
+      <c r="G138" s="2" t="n"/>
     </row>
     <row r="139" ht="12.75" customHeight="1">
-      <c r="A139" s="3" t="inlineStr">
+      <c r="A139" s="2" t="inlineStr">
         <is>
           <t>אוליבין ילנה</t>
         </is>
       </c>
-      <c r="B139" s="3" t="inlineStr">
+      <c r="B139" s="2" t="inlineStr">
         <is>
           <t>10/8</t>
         </is>
       </c>
-      <c r="G139" s="3" t="n"/>
+      <c r="G139" s="2" t="n"/>
     </row>
     <row r="140" ht="12.75" customHeight="1">
-      <c r="A140" s="3" t="inlineStr">
+      <c r="A140" s="2" t="inlineStr">
         <is>
           <t>קריגר איב</t>
         </is>
       </c>
-      <c r="B140" s="3" t="inlineStr">
+      <c r="B140" s="2" t="inlineStr">
         <is>
           <t>10/8</t>
         </is>
       </c>
-      <c r="G140" s="3" t="n"/>
+      <c r="G140" s="2" t="n"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
-      <c r="A141" s="3" t="inlineStr">
+      <c r="A141" s="2" t="inlineStr">
         <is>
           <t>קהלני ענת</t>
         </is>
       </c>
-      <c r="B141" s="3" t="inlineStr">
+      <c r="B141" s="2" t="inlineStr">
         <is>
           <t>14/8</t>
         </is>
       </c>
-      <c r="G141" s="3" t="n"/>
+      <c r="G141" s="2" t="n"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
-      <c r="A142" s="3" t="inlineStr">
+      <c r="A142" s="2" t="inlineStr">
         <is>
           <t>קמכדגי אמילי</t>
         </is>
       </c>
-      <c r="B142" s="3" t="inlineStr">
+      <c r="B142" s="2" t="inlineStr">
         <is>
           <t>14/8</t>
         </is>
       </c>
-      <c r="G142" s="3" t="n"/>
+      <c r="G142" s="2" t="n"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
-      <c r="A143" s="3" t="inlineStr">
+      <c r="A143" s="2" t="inlineStr">
         <is>
           <t>גלבוע רינה</t>
         </is>
       </c>
-      <c r="B143" s="3" t="inlineStr">
+      <c r="B143" s="2" t="inlineStr">
         <is>
           <t>15/8</t>
         </is>
       </c>
-      <c r="G143" s="3" t="n"/>
+      <c r="G143" s="2" t="n"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
-      <c r="A144" s="3" t="inlineStr">
+      <c r="A144" s="2" t="inlineStr">
         <is>
           <t>כהן חנוך חי</t>
         </is>
       </c>
-      <c r="B144" s="3" t="inlineStr">
+      <c r="B144" s="2" t="inlineStr">
         <is>
           <t>18/8</t>
         </is>
       </c>
-      <c r="G144" s="3" t="n"/>
+      <c r="G144" s="2" t="n"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
-      <c r="A145" s="3" t="inlineStr">
+      <c r="A145" s="2" t="inlineStr">
         <is>
           <t>קונסנס ורד</t>
         </is>
       </c>
-      <c r="B145" s="3" t="inlineStr">
+      <c r="B145" s="2" t="inlineStr">
         <is>
           <t>18/8</t>
         </is>
       </c>
-      <c r="G145" s="3" t="n"/>
+      <c r="G145" s="2" t="n"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
-      <c r="A146" s="3" t="inlineStr">
+      <c r="A146" s="2" t="inlineStr">
         <is>
           <t>לאמעי נורית</t>
         </is>
       </c>
-      <c r="B146" s="3" t="inlineStr">
+      <c r="B146" s="2" t="inlineStr">
         <is>
           <t>20/8</t>
         </is>
       </c>
-      <c r="G146" s="3" t="n"/>
+      <c r="G146" s="2" t="n"/>
     </row>
     <row r="147" ht="12.75" customHeight="1">
-      <c r="A147" s="3" t="inlineStr">
+      <c r="A147" s="2" t="inlineStr">
         <is>
           <t>גולריז שרון</t>
         </is>
       </c>
-      <c r="B147" s="3" t="inlineStr">
+      <c r="B147" s="2" t="inlineStr">
         <is>
           <t>24/8</t>
         </is>
       </c>
-      <c r="G147" s="3" t="n"/>
+      <c r="G147" s="2" t="n"/>
     </row>
     <row r="148" ht="12.75" customHeight="1">
-      <c r="A148" s="3" t="inlineStr">
+      <c r="A148" s="2" t="inlineStr">
         <is>
           <t>כבשנה ברטל צור</t>
         </is>
       </c>
-      <c r="B148" s="3" t="inlineStr">
+      <c r="B148" s="2" t="inlineStr">
         <is>
           <t>25/8</t>
         </is>
       </c>
-      <c r="G148" s="3" t="n"/>
+      <c r="G148" s="2" t="n"/>
     </row>
     <row r="149" ht="12.75" customHeight="1">
-      <c r="A149" s="3" t="inlineStr">
+      <c r="A149" s="2" t="inlineStr">
         <is>
           <t>כדורי ריטה</t>
         </is>
       </c>
-      <c r="B149" s="3" t="inlineStr">
+      <c r="B149" s="2" t="inlineStr">
         <is>
           <t>26/8</t>
         </is>
       </c>
-      <c r="G149" s="3" t="n"/>
+      <c r="G149" s="2" t="n"/>
     </row>
     <row r="150" ht="12.75" customHeight="1">
-      <c r="A150" s="3" t="inlineStr">
+      <c r="A150" s="2" t="inlineStr">
         <is>
           <t>דוד פורמן ליאת</t>
         </is>
       </c>
-      <c r="B150" s="3" t="inlineStr">
+      <c r="B150" s="2" t="inlineStr">
         <is>
           <t>27/8</t>
         </is>
       </c>
-      <c r="G150" s="3" t="n"/>
+      <c r="G150" s="2" t="n"/>
     </row>
     <row r="151" ht="12.75" customHeight="1">
-      <c r="A151" s="3" t="inlineStr">
+      <c r="A151" s="2" t="inlineStr">
         <is>
           <t>שושן ליאורה</t>
         </is>
       </c>
-      <c r="B151" s="3" t="inlineStr">
+      <c r="B151" s="2" t="inlineStr">
         <is>
           <t>28/8</t>
         </is>
       </c>
-      <c r="G151" s="3" t="n"/>
+      <c r="G151" s="2" t="n"/>
     </row>
     <row r="152" ht="12.75" customHeight="1">
-      <c r="A152" s="3" t="inlineStr">
+      <c r="A152" s="2" t="inlineStr">
         <is>
           <t>בן עמי ניצן מיכל</t>
         </is>
       </c>
-      <c r="B152" s="3" t="inlineStr">
+      <c r="B152" s="2" t="inlineStr">
         <is>
           <t>28/8</t>
         </is>
       </c>
-      <c r="G152" s="3" t="n"/>
+      <c r="G152" s="2" t="n"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
-      <c r="A153" s="3" t="inlineStr">
+      <c r="A153" s="2" t="inlineStr">
         <is>
           <t>פרץ דלית</t>
         </is>
       </c>
-      <c r="B153" s="3" t="inlineStr">
+      <c r="B153" s="2" t="inlineStr">
         <is>
           <t>29/8</t>
         </is>
       </c>
-      <c r="G153" s="3" t="n"/>
+      <c r="G153" s="2" t="n"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
-      <c r="A154" s="3" t="inlineStr">
+      <c r="A154" s="2" t="inlineStr">
         <is>
           <t>אלחורי בדיעה-בטי</t>
         </is>
       </c>
-      <c r="B154" s="3" t="inlineStr">
+      <c r="B154" s="2" t="inlineStr">
         <is>
           <t>30/8</t>
         </is>
       </c>
-      <c r="G154" s="3" t="n"/>
+      <c r="G154" s="2" t="n"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
-      <c r="A155" s="3" t="inlineStr">
+      <c r="A155" s="2" t="inlineStr">
         <is>
           <t>פרי קרן</t>
         </is>
       </c>
-      <c r="B155" s="3" t="inlineStr">
+      <c r="B155" s="2" t="inlineStr">
         <is>
           <t>31/8</t>
         </is>
       </c>
-      <c r="G155" s="3" t="n"/>
+      <c r="G155" s="2" t="n"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
       <c r="A156" t="inlineStr">
         <is>
+          <t>שפיגלמן</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+    </row>
+    <row r="157" ht="12.75" customHeight="1">
+      <c r="A157" t="inlineStr">
+        <is>
           <t>עידו קדם</t>
         </is>
       </c>
-      <c r="B156" t="inlineStr">
-        <is>
-          <t>12/05</t>
-        </is>
-      </c>
-    </row>
-    <row r="157" ht="12.75" customHeight="1"/>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>01/01</t>
+        </is>
+      </c>
+    </row>
     <row r="158" ht="12.75" customHeight="1"/>
     <row r="159" ht="12.75" customHeight="1"/>
     <row r="160" ht="12.75" customHeight="1"/>

</xml_diff>